<commit_message>
Changes to add plots
</commit_message>
<xml_diff>
--- a/Data/Data_Dictionary.xlsx
+++ b/Data/Data_Dictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohit/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\general\Downloads\OneDrive - ARRIS Group, Inc\Upgrad\Module-2\Group Case Study\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -21,9 +21,6 @@
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1362,7 +1359,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1396,6 +1393,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="92">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1819,25 +1827,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="196.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>94</v>
       </c>
@@ -1845,7 +1853,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>229</v>
       </c>
@@ -1854,7 +1862,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>233</v>
       </c>
@@ -1863,7 +1871,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1872,7 +1880,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>223</v>
       </c>
@@ -1881,7 +1889,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1890,7 +1898,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>191</v>
       </c>
@@ -1899,7 +1907,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>189</v>
       </c>
@@ -1908,7 +1916,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>108</v>
       </c>
@@ -1917,7 +1925,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>234</v>
       </c>
@@ -1926,7 +1934,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>235</v>
       </c>
@@ -1935,7 +1943,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>99</v>
       </c>
@@ -1944,7 +1952,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>165</v>
       </c>
@@ -1953,7 +1961,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>100</v>
       </c>
@@ -1962,7 +1970,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1971,7 +1979,7 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>236</v>
       </c>
@@ -1980,7 +1988,7 @@
       </c>
       <c r="C16" s="20"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -1989,16 +1997,16 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>192</v>
       </c>
@@ -2007,7 +2015,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2016,7 +2024,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2025,7 +2033,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>154</v>
       </c>
@@ -2034,7 +2042,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2043,7 +2051,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2052,7 +2060,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2061,7 +2069,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2070,7 +2078,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -2079,7 +2087,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2096,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2097,7 +2105,7 @@
       </c>
       <c r="C29" s="20"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>215</v>
       </c>
@@ -2106,7 +2114,7 @@
       </c>
       <c r="C30" s="20"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2115,7 +2123,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>225</v>
       </c>
@@ -2124,7 +2132,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>227</v>
       </c>
@@ -2133,7 +2141,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2142,7 +2150,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2151,7 +2159,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2160,7 +2168,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2171,7 +2179,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2180,7 +2188,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2189,7 +2197,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2198,7 +2206,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2207,7 +2215,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2216,7 +2224,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2225,7 +2233,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2234,7 +2242,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>221</v>
       </c>
@@ -2243,7 +2251,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2255,7 +2263,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>237</v>
       </c>
@@ -2267,7 +2275,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>118</v>
       </c>
@@ -2279,7 +2287,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>119</v>
       </c>
@@ -2288,7 +2296,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>105</v>
       </c>
@@ -2297,7 +2305,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>238</v>
       </c>
@@ -2306,7 +2314,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2315,7 +2323,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>102</v>
       </c>
@@ -2324,16 +2332,17 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="23"/>
+      <c r="D54" s="24"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>211</v>
       </c>
@@ -2342,7 +2351,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>239</v>
       </c>
@@ -2351,7 +2360,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>240</v>
       </c>
@@ -2360,7 +2369,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>242</v>
       </c>
@@ -2369,7 +2378,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>243</v>
       </c>
@@ -2378,7 +2387,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2387,7 +2396,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>98</v>
       </c>
@@ -2396,7 +2405,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>110</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -2412,7 +2421,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>111</v>
       </c>
@@ -2420,7 +2429,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>109</v>
       </c>
@@ -2428,7 +2437,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>116</v>
       </c>
@@ -2436,7 +2445,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>121</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>96</v>
       </c>
@@ -2452,7 +2461,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>120</v>
       </c>
@@ -2460,7 +2469,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>103</v>
       </c>
@@ -2468,7 +2477,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>115</v>
       </c>
@@ -2476,7 +2485,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>114</v>
       </c>
@@ -2484,7 +2493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>113</v>
       </c>
@@ -2494,7 +2503,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>104</v>
       </c>
@@ -2502,7 +2511,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2510,7 +2519,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>203</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>207</v>
       </c>
@@ -2526,7 +2535,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>209</v>
       </c>
@@ -2534,7 +2543,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>205</v>
       </c>
@@ -2542,7 +2551,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>217</v>
       </c>
@@ -2550,7 +2559,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>219</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -2566,7 +2575,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -2574,7 +2583,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>112</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>244</v>
       </c>
@@ -2590,7 +2599,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>123</v>
       </c>
@@ -2598,7 +2607,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>97</v>
       </c>
@@ -2614,7 +2623,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>18</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -2630,7 +2639,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>164</v>
       </c>
@@ -2638,7 +2647,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -2646,7 +2655,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -2654,7 +2663,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -2662,7 +2671,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>101</v>
       </c>
@@ -2670,7 +2679,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -2678,7 +2687,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2695,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>122</v>
       </c>
@@ -2694,7 +2703,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>107</v>
       </c>
@@ -2702,7 +2711,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>106</v>
       </c>
@@ -2710,7 +2719,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -2718,7 +2727,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>245</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>213</v>
       </c>
@@ -2734,7 +2743,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>246</v>
       </c>
@@ -2742,7 +2751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>231</v>
       </c>
@@ -2750,7 +2759,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>95</v>
       </c>
@@ -2758,7 +2767,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -2766,7 +2775,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -2774,7 +2783,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -2790,7 +2799,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -2798,7 +2807,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>158</v>
       </c>
@@ -2806,7 +2815,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -2814,7 +2823,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>232</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>194</v>
       </c>
@@ -2830,7 +2839,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
         <v>184</v>
       </c>
@@ -2838,7 +2847,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B118" s="13" t="s">
         <v>156</v>
       </c>
@@ -2853,7 +2862,7 @@
     <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
+  <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2865,13 +2874,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>166</v>
       </c>
@@ -2879,7 +2888,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>167</v>
       </c>
@@ -2887,7 +2896,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>168</v>
       </c>
@@ -2895,7 +2904,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>169</v>
       </c>
@@ -2903,7 +2912,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>180</v>
       </c>
@@ -2911,7 +2920,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>170</v>
       </c>
@@ -2919,7 +2928,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>182</v>
       </c>
@@ -2927,7 +2936,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>171</v>
       </c>
@@ -2935,7 +2944,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>172</v>
       </c>
@@ -2943,7 +2952,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>173</v>
       </c>
@@ -2951,11 +2960,11 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="19"/>
     </row>

</xml_diff>